<commit_message>
generatpr settings and user david
</commit_message>
<xml_diff>
--- a/algorithm/shifts.xlsx
+++ b/algorithm/shifts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B1" t="n">
@@ -432,22 +432,22 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E1" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -455,22 +455,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,12 +478,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -493,7 +493,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -501,22 +501,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -524,7 +524,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -533,13 +533,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -547,22 +547,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -570,12 +570,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -585,7 +585,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -593,22 +593,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
       <c r="E8" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -631,7 +631,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -639,12 +639,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -654,7 +654,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -667,17 +667,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -685,22 +685,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -708,22 +708,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -731,22 +731,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -754,12 +754,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -769,7 +769,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -777,12 +777,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -792,7 +792,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -800,22 +800,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -823,12 +823,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -838,7 +838,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -846,22 +846,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -869,12 +869,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -884,7 +884,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -892,12 +892,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -907,7 +907,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -915,22 +915,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -938,22 +938,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Doctor</t>
+          <t>Cashier</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -966,17 +966,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -984,12 +984,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -999,7 +999,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1007,22 +1007,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E26" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1030,22 +1030,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1053,22 +1053,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1076,22 +1076,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1099,22 +1099,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1122,12 +1122,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1137,7 +1137,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1145,12 +1145,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1160,7 +1160,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1168,12 +1168,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1183,7 +1183,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1191,12 +1191,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1206,7 +1206,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1214,12 +1214,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1229,7 +1229,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1237,12 +1237,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1252,7 +1252,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1260,12 +1260,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1275,7 +1275,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1283,22 +1283,22 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1306,12 +1306,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1321,7 +1321,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1329,12 +1329,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1344,7 +1344,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1357,17 +1357,17 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1375,22 +1375,22 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1398,12 +1398,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1413,7 +1413,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1421,12 +1421,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1436,7 +1436,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1444,12 +1444,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>13:00</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>18:00</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1459,7 +1459,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1467,12 +1467,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1482,7 +1482,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1490,22 +1490,22 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Stock Clerk</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1518,17 +1518,17 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
           <t>14:00</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>19:00</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1551,7 +1551,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1559,22 +1559,22 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1582,22 +1582,22 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1605,22 +1605,22 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1637,13 +1637,13 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1660,13 +1660,13 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1674,12 +1674,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1689,7 +1689,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1697,12 +1697,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -1712,7 +1712,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1720,22 +1720,22 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1743,22 +1743,22 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1766,22 +1766,22 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1794,17 +1794,17 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1812,12 +1812,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -1827,7 +1827,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1835,22 +1835,22 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1858,12 +1858,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -1873,7 +1873,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1881,12 +1881,12 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -1896,7 +1896,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1919,7 +1919,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1927,12 +1927,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -1942,7 +1942,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1950,22 +1950,22 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
       <c r="E67" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1973,12 +1973,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -1988,7 +1988,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1996,12 +1996,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2011,7 +2011,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -2019,12 +2019,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2034,7 +2034,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -2042,22 +2042,22 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Nurse</t>
+          <t>Customer Service</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -2075,558 +2075,6 @@
       </c>
       <c r="E72" t="n">
         <v>60</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>1</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>1</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="E76" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>2</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>2</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="E79" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B80" t="n">
-        <v>2</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B81" t="n">
-        <v>3</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>3</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B83" t="n">
-        <v>3</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E83" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>3</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E84" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B85" t="n">
-        <v>4</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="E85" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B86" t="n">
-        <v>4</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="E86" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B87" t="n">
-        <v>4</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="E87" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
-        <v>4</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="E88" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B89" t="n">
-        <v>5</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="E89" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B90" t="n">
-        <v>5</v>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="E90" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B91" t="n">
-        <v>5</v>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="E91" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>5</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="E92" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v>6</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="E93" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>6</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="E94" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B95" t="n">
-        <v>6</v>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="E95" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v>6</v>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="E96" t="n">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>